<commit_message>
new charts in Appendix 2
</commit_message>
<xml_diff>
--- a/R/Dated_inscriptions_coefficient.xlsx
+++ b/R/Dated_inscriptions_coefficient.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -107,17 +108,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="0.00%"/>
-    <numFmt numFmtId="167" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -138,14 +139,28 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -232,7 +247,7 @@
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF7E0021"/>
+      <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
@@ -245,8 +260,8 @@
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF6666"/>
-      <rgbColor rgb="FF0084D1"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
@@ -264,10 +279,10 @@
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF3399FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FFAECF00"/>
-      <rgbColor rgb="FFFFD320"/>
+      <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF420E"/>
       <rgbColor rgb="FF666699"/>
@@ -285,7 +300,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -330,8 +345,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0247409205489683"/>
-          <c:y val="0.0258279082932352"/>
+          <c:x val="0.0247381640680536"/>
+          <c:y val="0.0258986696858194"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -366,6 +381,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -466,14 +482,14 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.66</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="7e0021"/>
+              <a:srgbClr val="ff8080"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -481,6 +497,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -536,37 +553,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>63.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>74.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>90.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>138</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>103.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -581,14 +598,14 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.5</c:v>
+                  <c:v>0.33</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="ff6666"/>
+              <a:srgbClr val="0000ff"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -596,6 +613,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -651,37 +669,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>63.5</c:v>
+                  <c:v>0.333333333333333</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>74.5</c:v>
+                  <c:v>1.66666666666667</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42</c:v>
+                  <c:v>3.66666666666667</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>92</c:v>
+                  <c:v>4.66666666666667</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>90.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>75</c:v>
+                  <c:v>15.3333333333333</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>138</c:v>
+                  <c:v>14.3333333333333</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>103.5</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>30</c:v>
+                  <c:v>14.6666666666667</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>18</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -696,14 +714,14 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.33</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="0084d1"/>
+              <a:srgbClr val="3399ff"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -711,6 +729,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -769,34 +788,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.333333333333333</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.66666666666667</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.66666666666667</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.66666666666667</c:v>
+                  <c:v>10.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15.3333333333333</c:v>
+                  <c:v>30.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14.3333333333333</c:v>
+                  <c:v>20.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>29</c:v>
+                  <c:v>20.75</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14.6666666666667</c:v>
+                  <c:v>20.75</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -811,7 +830,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.25</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -826,6 +845,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -884,34 +904,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.25</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10.5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10.25</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>30.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>20.25</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>20.75</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>20.75</c:v>
-                </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.75</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -926,7 +946,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.2</c:v>
+                  <c:v>0.16</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -941,6 +961,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -999,34 +1020,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.4</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.2</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.2</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.2</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1041,7 +1062,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.16</c:v>
+                  <c:v>0.125</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1056,6 +1077,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1120,121 +1142,6 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="7"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$I$17</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.125</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ffd320"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$18:$A$28</c:f>
-              <c:strCache>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>6 st. př. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5 st. př. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4 st. př. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3 st. př. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2 st. př. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1 st. př. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1 st. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2 st. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3 st. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4 st. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5 st. n. l.</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$I$18:$I$28</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>0.142857142857143</c:v>
                 </c:pt>
                 <c:pt idx="4">
@@ -1264,11 +1171,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="74605330"/>
-        <c:axId val="87298115"/>
+        <c:axId val="70172118"/>
+        <c:axId val="46014137"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="74605330"/>
+        <c:axId val="70172118"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1341,14 +1248,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="87298115"/>
+        <c:crossAx val="46014137"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="87298115"/>
+        <c:axId val="46014137"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1401,7 +1308,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1430,7 +1337,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74605330"/>
+        <c:crossAx val="70172118"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1472,15 +1379,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>88920</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>19440</xdr:rowOff>
+      <xdr:colOff>553320</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>143640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>485280</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>67320</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>148320</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>28800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1488,8 +1395,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9029520" y="2457720"/>
-        <a:ext cx="7711560" cy="5087160"/>
+        <a:off x="9354240" y="2256840"/>
+        <a:ext cx="7596000" cy="5087160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1507,15 +1414,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:M28"/>
+  <dimension ref="A2:L28"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O13" activeCellId="0" sqref="O13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S50" activeCellId="0" sqref="S50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1526,34 +1433,31 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>0.66</v>
+        <v>0.5</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>0.5</v>
+        <v>0.33</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="G2" s="1" t="n">
-        <v>0.2</v>
+        <v>0.16</v>
       </c>
       <c r="H2" s="1" t="n">
-        <v>0.16</v>
-      </c>
-      <c r="I2" s="1" t="n">
         <v>0.125</v>
       </c>
+      <c r="I2" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="J2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="2"/>
-      <c r="M2" s="1" t="s">
+      <c r="K2" s="2"/>
+      <c r="L2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1565,10 +1469,10 @@
         <v>3</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>0</v>
@@ -1583,18 +1487,15 @@
         <v>0</v>
       </c>
       <c r="I3" s="1" t="n">
-        <v>0</v>
+        <v>7.16</v>
       </c>
       <c r="J3" s="1" t="n">
-        <v>7.16</v>
-      </c>
-      <c r="K3" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="1" t="n">
+      <c r="L3" s="1" t="n">
         <v>8</v>
       </c>
     </row>
@@ -1606,10 +1507,10 @@
         <v>60</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>127</v>
+        <v>1</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>1</v>
@@ -1618,24 +1519,21 @@
         <v>1</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>0</v>
+        <v>170.05</v>
       </c>
       <c r="J4" s="1" t="n">
-        <v>170.05</v>
-      </c>
-      <c r="K4" s="1" t="n">
         <v>187</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="1" t="n">
+      <c r="L4" s="1" t="n">
         <v>190</v>
       </c>
     </row>
@@ -1647,36 +1545,33 @@
         <v>168</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>0</v>
+        <v>149</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>149</v>
+        <v>5</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="G5" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I5" s="1" t="n">
-        <v>0</v>
+        <v>326.675</v>
       </c>
       <c r="J5" s="1" t="n">
-        <v>326.675</v>
-      </c>
-      <c r="K5" s="1" t="n">
         <v>317</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="K5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M5" s="1" t="n">
+      <c r="L5" s="1" t="n">
         <v>365</v>
       </c>
     </row>
@@ -1688,36 +1583,33 @@
         <v>117</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>84</v>
+        <v>11</v>
       </c>
       <c r="E6" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>228.225</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <v>201</v>
+      </c>
+      <c r="K6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="1" t="n">
-        <v>41</v>
-      </c>
-      <c r="G6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J6" s="1" t="n">
-        <v>228.225</v>
-      </c>
-      <c r="K6" s="1" t="n">
-        <v>201</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M6" s="1" t="n">
+      <c r="L6" s="1" t="n">
         <v>255</v>
       </c>
     </row>
@@ -1729,36 +1621,33 @@
         <v>115</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>0</v>
+        <v>184</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>184</v>
+        <v>14</v>
       </c>
       <c r="E7" s="1" t="n">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="G7" s="1" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H7" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" s="1" t="n">
-        <v>1</v>
+        <v>320.41</v>
       </c>
       <c r="J7" s="1" t="n">
-        <v>320.41</v>
-      </c>
-      <c r="K7" s="1" t="n">
         <v>299</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="K7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="1" t="n">
+      <c r="L7" s="1" t="n">
         <v>358</v>
       </c>
     </row>
@@ -1770,36 +1659,33 @@
         <v>69</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>0</v>
+        <v>181</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>181</v>
+        <v>9</v>
       </c>
       <c r="E8" s="1" t="n">
+        <v>122</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="F8" s="1" t="n">
-        <v>122</v>
-      </c>
-      <c r="G8" s="1" t="n">
-        <v>2</v>
-      </c>
       <c r="H8" s="1" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I8" s="1" t="n">
-        <v>1</v>
+        <v>351.735</v>
       </c>
       <c r="J8" s="1" t="n">
-        <v>351.735</v>
-      </c>
-      <c r="K8" s="1" t="n">
         <v>250</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="K8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="M8" s="1" t="n">
+      <c r="L8" s="1" t="n">
         <v>393</v>
       </c>
     </row>
@@ -1811,36 +1697,33 @@
         <v>68</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>150</v>
+        <v>46</v>
       </c>
       <c r="E9" s="1" t="n">
-        <v>46</v>
+        <v>81</v>
       </c>
       <c r="F9" s="1" t="n">
-        <v>81</v>
+        <v>1</v>
       </c>
       <c r="G9" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="H9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="H9" s="1" t="n">
-        <v>9</v>
-      </c>
       <c r="I9" s="1" t="n">
-        <v>1</v>
+        <v>318.62</v>
       </c>
       <c r="J9" s="1" t="n">
-        <v>318.62</v>
-      </c>
-      <c r="K9" s="1" t="n">
         <v>218</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="K9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="M9" s="1" t="n">
+      <c r="L9" s="1" t="n">
         <v>356</v>
       </c>
     </row>
@@ -1852,36 +1735,33 @@
         <v>253</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>0</v>
+        <v>276</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>276</v>
+        <v>43</v>
       </c>
       <c r="E10" s="1" t="n">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="F10" s="1" t="n">
-        <v>83</v>
+        <v>1</v>
       </c>
       <c r="G10" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="H10" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="H10" s="1" t="n">
-        <v>9</v>
-      </c>
       <c r="I10" s="1" t="n">
-        <v>1</v>
+        <v>596.07</v>
       </c>
       <c r="J10" s="1" t="n">
-        <v>596.07</v>
-      </c>
-      <c r="K10" s="1" t="n">
         <v>529</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="K10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M10" s="1" t="n">
+      <c r="L10" s="1" t="n">
         <v>666</v>
       </c>
     </row>
@@ -1893,36 +1773,33 @@
         <v>390</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>0</v>
+        <v>207</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>207</v>
+        <v>87</v>
       </c>
       <c r="E11" s="1" t="n">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F11" s="1" t="n">
-        <v>83</v>
+        <v>1</v>
       </c>
       <c r="G11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="H11" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="H11" s="1" t="n">
-        <v>9</v>
-      </c>
       <c r="I11" s="1" t="n">
-        <v>1</v>
+        <v>696.31</v>
       </c>
       <c r="J11" s="1" t="n">
-        <v>696.31</v>
-      </c>
-      <c r="K11" s="1" t="n">
         <v>597</v>
       </c>
-      <c r="L11" s="3" t="s">
+      <c r="K11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="M11" s="1" t="n">
+      <c r="L11" s="1" t="n">
         <v>778</v>
       </c>
     </row>
@@ -1934,36 +1811,33 @@
         <v>23</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="E12" s="1" t="n">
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="F12" s="1" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H12" s="1" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I12" s="1" t="n">
-        <v>1</v>
+        <v>125.3</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>125.3</v>
-      </c>
-      <c r="K12" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="L12" s="3" t="s">
+      <c r="K12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="M12" s="1" t="n">
+      <c r="L12" s="1" t="n">
         <v>140</v>
       </c>
     </row>
@@ -1975,36 +1849,33 @@
         <v>42</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="E13" s="1" t="n">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="F13" s="1" t="n">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H13" s="1" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I13" s="1" t="n">
-        <v>1</v>
+        <v>118.14</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>118.14</v>
-      </c>
-      <c r="K13" s="1" t="n">
         <v>78</v>
       </c>
-      <c r="L13" s="3" t="s">
+      <c r="K13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M13" s="1" t="n">
+      <c r="L13" s="1" t="n">
         <v>132</v>
       </c>
     </row>
@@ -2013,8 +1884,8 @@
         <f aca="false">SUM(B2:B13)</f>
         <v>1309</v>
       </c>
-      <c r="D14" s="0" t="n">
-        <f aca="false">SUM(D3:D13)</f>
+      <c r="C14" s="0" t="n">
+        <f aca="false">SUM(C3:C13)</f>
         <v>1458</v>
       </c>
     </row>
@@ -2026,33 +1897,30 @@
         <v>1</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>0.66</v>
+        <v>0.5</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>0.5</v>
+        <v>0.33</v>
       </c>
       <c r="E17" s="1" t="n">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="F17" s="1" t="n">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="G17" s="1" t="n">
-        <v>0.2</v>
+        <v>0.16</v>
       </c>
       <c r="H17" s="1" t="n">
-        <v>0.16</v>
-      </c>
-      <c r="I17" s="1" t="n">
         <v>0.125</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="I17" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="J17" s="0" t="s">
+        <v>26</v>
+      </c>
       <c r="K17" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="L17" s="0" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2064,38 +1932,34 @@
         <v>3</v>
       </c>
       <c r="C18" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <f aca="false">D3/3</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <f aca="false">B18+C18</f>
+        <v>6</v>
+      </c>
+      <c r="J18" s="4" t="n">
+        <f aca="false">I18/K18</f>
         <v>1</v>
       </c>
-      <c r="D18" s="1" t="n">
-        <f aca="false">D3/2</f>
-        <v>2</v>
-      </c>
-      <c r="E18" s="1" t="n">
-        <f aca="false">E3/3</f>
-        <v>0</v>
-      </c>
-      <c r="F18" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G18" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H18" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I18" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J18" s="0" t="n">
-        <f aca="false">B18+C18+D18</f>
-        <v>6</v>
-      </c>
-      <c r="K18" s="4" t="n">
-        <f aca="false">J18/L18</f>
-        <v>1</v>
-      </c>
-      <c r="L18" s="0" t="n">
-        <f aca="false">SUM(B18:I18)</f>
+      <c r="K18" s="0" t="n">
+        <f aca="false">SUM(B18:H18)</f>
         <v>6</v>
       </c>
     </row>
@@ -2107,42 +1971,39 @@
         <v>60</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>0</v>
+        <f aca="false">C4/2</f>
+        <v>63.5</v>
       </c>
       <c r="D19" s="1" t="n">
-        <f aca="false">D4/2</f>
-        <v>63.5</v>
+        <f aca="false">D4/3</f>
+        <v>0.333333333333333</v>
       </c>
       <c r="E19" s="1" t="n">
-        <f aca="false">E4/3</f>
-        <v>0.333333333333333</v>
+        <f aca="false">E3/4</f>
+        <v>0</v>
       </c>
       <c r="F19" s="1" t="n">
-        <f aca="false">F3/4</f>
-        <v>0</v>
+        <f aca="false">F4/5</f>
+        <v>0.2</v>
       </c>
       <c r="G19" s="1" t="n">
-        <f aca="false">G4/5</f>
-        <v>0.2</v>
+        <f aca="false">G4/6</f>
+        <v>0</v>
       </c>
       <c r="H19" s="1" t="n">
-        <f aca="false">H4/6</f>
-        <v>0</v>
-      </c>
-      <c r="I19" s="1" t="n">
-        <f aca="false">I4/7</f>
-        <v>0</v>
-      </c>
-      <c r="J19" s="0" t="n">
-        <f aca="false">B19+C19+D19</f>
+        <f aca="false">H4/7</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <f aca="false">B19+C19</f>
         <v>123.5</v>
       </c>
-      <c r="K19" s="4" t="n">
-        <f aca="false">J19/L19</f>
+      <c r="J19" s="4" t="n">
+        <f aca="false">I19/K19</f>
         <v>0.995700080623488</v>
       </c>
-      <c r="L19" s="0" t="n">
-        <f aca="false">SUM(B19:I19)</f>
+      <c r="K19" s="0" t="n">
+        <f aca="false">SUM(B19:H19)</f>
         <v>124.033333333333</v>
       </c>
     </row>
@@ -2154,42 +2015,39 @@
         <v>168</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>0</v>
+        <f aca="false">C5/2</f>
+        <v>74.5</v>
       </c>
       <c r="D20" s="1" t="n">
-        <f aca="false">D5/2</f>
-        <v>74.5</v>
+        <f aca="false">D5/3</f>
+        <v>1.66666666666667</v>
       </c>
       <c r="E20" s="1" t="n">
-        <f aca="false">E5/3</f>
-        <v>1.66666666666667</v>
+        <f aca="false">E4/4</f>
+        <v>0.25</v>
       </c>
       <c r="F20" s="1" t="n">
-        <f aca="false">F4/4</f>
-        <v>0.25</v>
+        <f aca="false">F5/5</f>
+        <v>0.2</v>
       </c>
       <c r="G20" s="1" t="n">
-        <f aca="false">G5/5</f>
-        <v>0.2</v>
+        <f aca="false">G5/6</f>
+        <v>0</v>
       </c>
       <c r="H20" s="1" t="n">
-        <f aca="false">H5/6</f>
-        <v>0</v>
-      </c>
-      <c r="I20" s="1" t="n">
-        <f aca="false">I5/7</f>
-        <v>0</v>
-      </c>
-      <c r="J20" s="0" t="n">
-        <f aca="false">B20+C20+D20</f>
+        <f aca="false">H5/7</f>
+        <v>0</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <f aca="false">B20+C20</f>
         <v>242.5</v>
       </c>
-      <c r="K20" s="4" t="n">
-        <f aca="false">J20/L20</f>
+      <c r="J20" s="4" t="n">
+        <f aca="false">I20/K20</f>
         <v>0.991347005518839</v>
       </c>
-      <c r="L20" s="0" t="n">
-        <f aca="false">SUM(B20:I20)</f>
+      <c r="K20" s="0" t="n">
+        <f aca="false">SUM(B20:H20)</f>
         <v>244.616666666667</v>
       </c>
     </row>
@@ -2201,42 +2059,39 @@
         <v>117</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>0</v>
+        <f aca="false">C6/2</f>
+        <v>42</v>
       </c>
       <c r="D21" s="1" t="n">
-        <f aca="false">D6/2</f>
-        <v>42</v>
+        <f aca="false">D6/3</f>
+        <v>3.66666666666667</v>
       </c>
       <c r="E21" s="1" t="n">
-        <f aca="false">E6/3</f>
-        <v>3.66666666666667</v>
+        <f aca="false">E5/4</f>
+        <v>10.5</v>
       </c>
       <c r="F21" s="1" t="n">
-        <f aca="false">F5/4</f>
-        <v>10.5</v>
+        <f aca="false">F6/5</f>
+        <v>0.2</v>
       </c>
       <c r="G21" s="1" t="n">
-        <f aca="false">G6/5</f>
-        <v>0.2</v>
+        <f aca="false">G6/6</f>
+        <v>0</v>
       </c>
       <c r="H21" s="1" t="n">
-        <f aca="false">H6/6</f>
-        <v>0</v>
-      </c>
-      <c r="I21" s="1" t="n">
-        <f aca="false">I6/7</f>
+        <f aca="false">H6/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="J21" s="0" t="n">
-        <f aca="false">B21+C21+D21</f>
+      <c r="I21" s="0" t="n">
+        <f aca="false">B21+C21</f>
         <v>159</v>
       </c>
-      <c r="K21" s="4" t="n">
-        <f aca="false">J21/L21</f>
+      <c r="J21" s="4" t="n">
+        <f aca="false">I21/K21</f>
         <v>0.916376210994319</v>
       </c>
-      <c r="L21" s="0" t="n">
-        <f aca="false">SUM(B21:I21)</f>
+      <c r="K21" s="0" t="n">
+        <f aca="false">SUM(B21:H21)</f>
         <v>173.509523809524</v>
       </c>
     </row>
@@ -2248,42 +2103,39 @@
         <v>115</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>0</v>
+        <f aca="false">C7/2</f>
+        <v>92</v>
       </c>
       <c r="D22" s="1" t="n">
-        <f aca="false">D7/2</f>
-        <v>92</v>
+        <f aca="false">D7/3</f>
+        <v>4.66666666666667</v>
       </c>
       <c r="E22" s="1" t="n">
-        <f aca="false">E7/3</f>
-        <v>4.66666666666667</v>
+        <f aca="false">E6/4</f>
+        <v>10.25</v>
       </c>
       <c r="F22" s="1" t="n">
-        <f aca="false">F6/4</f>
-        <v>10.25</v>
+        <f aca="false">F7/5</f>
+        <v>0.4</v>
       </c>
       <c r="G22" s="1" t="n">
-        <f aca="false">G7/5</f>
-        <v>0.4</v>
+        <f aca="false">G7/6</f>
+        <v>0</v>
       </c>
       <c r="H22" s="1" t="n">
-        <f aca="false">H7/6</f>
-        <v>0</v>
-      </c>
-      <c r="I22" s="1" t="n">
-        <f aca="false">I7/7</f>
+        <f aca="false">H7/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="J22" s="0" t="n">
-        <f aca="false">B22+C22+D22</f>
+      <c r="I22" s="0" t="n">
+        <f aca="false">B22+C22</f>
         <v>207</v>
       </c>
-      <c r="K22" s="4" t="n">
-        <f aca="false">J22/L22</f>
+      <c r="J22" s="4" t="n">
+        <f aca="false">I22/K22</f>
         <v>0.930506352145387</v>
       </c>
-      <c r="L22" s="0" t="n">
-        <f aca="false">SUM(B22:I22)</f>
+      <c r="K22" s="0" t="n">
+        <f aca="false">SUM(B22:H22)</f>
         <v>222.459523809524</v>
       </c>
     </row>
@@ -2295,42 +2147,39 @@
         <v>69</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>0</v>
+        <f aca="false">C8/2</f>
+        <v>90.5</v>
       </c>
       <c r="D23" s="1" t="n">
-        <f aca="false">D8/2</f>
-        <v>90.5</v>
+        <f aca="false">D8/3</f>
+        <v>3</v>
       </c>
       <c r="E23" s="1" t="n">
-        <f aca="false">E8/3</f>
-        <v>3</v>
+        <f aca="false">E7/4</f>
+        <v>10.5</v>
       </c>
       <c r="F23" s="1" t="n">
-        <f aca="false">F7/4</f>
-        <v>10.5</v>
+        <f aca="false">F8/5</f>
+        <v>0.4</v>
       </c>
       <c r="G23" s="1" t="n">
-        <f aca="false">G8/5</f>
-        <v>0.4</v>
+        <f aca="false">G8/6</f>
+        <v>1.5</v>
       </c>
       <c r="H23" s="1" t="n">
-        <f aca="false">H8/6</f>
-        <v>1.5</v>
-      </c>
-      <c r="I23" s="1" t="n">
-        <f aca="false">I8/7</f>
+        <f aca="false">H8/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="J23" s="0" t="n">
-        <f aca="false">B23+C23+D23</f>
+      <c r="I23" s="0" t="n">
+        <f aca="false">B23+C23</f>
         <v>159.5</v>
       </c>
-      <c r="K23" s="4" t="n">
-        <f aca="false">J23/L23</f>
+      <c r="J23" s="4" t="n">
+        <f aca="false">I23/K23</f>
         <v>0.911205419081041</v>
       </c>
-      <c r="L23" s="0" t="n">
-        <f aca="false">SUM(B23:I23)</f>
+      <c r="K23" s="0" t="n">
+        <f aca="false">SUM(B23:H23)</f>
         <v>175.042857142857</v>
       </c>
     </row>
@@ -2342,42 +2191,39 @@
         <v>68</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>0</v>
+        <f aca="false">C9/2</f>
+        <v>75</v>
       </c>
       <c r="D24" s="1" t="n">
-        <f aca="false">D9/2</f>
-        <v>75</v>
+        <f aca="false">D9/3</f>
+        <v>15.3333333333333</v>
       </c>
       <c r="E24" s="1" t="n">
-        <f aca="false">E9/3</f>
-        <v>15.3333333333333</v>
+        <f aca="false">E8/4</f>
+        <v>30.5</v>
       </c>
       <c r="F24" s="1" t="n">
-        <f aca="false">F8/4</f>
-        <v>30.5</v>
+        <f aca="false">F9/5</f>
+        <v>0.2</v>
       </c>
       <c r="G24" s="1" t="n">
-        <f aca="false">G9/5</f>
-        <v>0.2</v>
+        <f aca="false">G9/6</f>
+        <v>1.5</v>
       </c>
       <c r="H24" s="1" t="n">
-        <f aca="false">H9/6</f>
-        <v>1.5</v>
-      </c>
-      <c r="I24" s="1" t="n">
-        <f aca="false">I9/7</f>
+        <f aca="false">H9/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="J24" s="0" t="n">
-        <f aca="false">B24+C24+D24</f>
+      <c r="I24" s="0" t="n">
+        <f aca="false">B24+C24</f>
         <v>143</v>
       </c>
-      <c r="K24" s="4" t="n">
-        <f aca="false">J24/L24</f>
+      <c r="J24" s="4" t="n">
+        <f aca="false">I24/K24</f>
         <v>0.7499625393337</v>
       </c>
-      <c r="L24" s="0" t="n">
-        <f aca="false">SUM(B24:I24)</f>
+      <c r="K24" s="0" t="n">
+        <f aca="false">SUM(B24:H24)</f>
         <v>190.67619047619</v>
       </c>
     </row>
@@ -2389,42 +2235,39 @@
         <v>253</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>0</v>
+        <f aca="false">C10/2</f>
+        <v>138</v>
       </c>
       <c r="D25" s="1" t="n">
-        <f aca="false">D10/2</f>
-        <v>138</v>
+        <f aca="false">D10/3</f>
+        <v>14.3333333333333</v>
       </c>
       <c r="E25" s="1" t="n">
-        <f aca="false">E10/3</f>
-        <v>14.3333333333333</v>
+        <f aca="false">E9/4</f>
+        <v>20.25</v>
       </c>
       <c r="F25" s="1" t="n">
-        <f aca="false">F9/4</f>
-        <v>20.25</v>
+        <f aca="false">F10/5</f>
+        <v>0.2</v>
       </c>
       <c r="G25" s="1" t="n">
-        <f aca="false">G10/5</f>
-        <v>0.2</v>
+        <f aca="false">G10/6</f>
+        <v>1.5</v>
       </c>
       <c r="H25" s="1" t="n">
-        <f aca="false">H10/6</f>
-        <v>1.5</v>
-      </c>
-      <c r="I25" s="1" t="n">
-        <f aca="false">I10/7</f>
+        <f aca="false">H10/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="J25" s="0" t="n">
-        <f aca="false">B25+C25+D25</f>
+      <c r="I25" s="0" t="n">
+        <f aca="false">B25+C25</f>
         <v>391</v>
       </c>
-      <c r="K25" s="4" t="n">
-        <f aca="false">J25/L25</f>
+      <c r="J25" s="4" t="n">
+        <f aca="false">I25/K25</f>
         <v>0.914777822960244</v>
       </c>
-      <c r="L25" s="0" t="n">
-        <f aca="false">SUM(B25:I25)</f>
+      <c r="K25" s="0" t="n">
+        <f aca="false">SUM(B25:H25)</f>
         <v>427.42619047619</v>
       </c>
     </row>
@@ -2436,42 +2279,39 @@
         <v>390</v>
       </c>
       <c r="C26" s="1" t="n">
-        <v>0</v>
+        <f aca="false">C11/2</f>
+        <v>103.5</v>
       </c>
       <c r="D26" s="1" t="n">
-        <f aca="false">D11/2</f>
-        <v>103.5</v>
+        <f aca="false">D11/3</f>
+        <v>29</v>
       </c>
       <c r="E26" s="1" t="n">
-        <f aca="false">E11/3</f>
-        <v>29</v>
+        <f aca="false">E10/4</f>
+        <v>20.75</v>
       </c>
       <c r="F26" s="1" t="n">
-        <f aca="false">F10/4</f>
-        <v>20.75</v>
+        <f aca="false">F11/5</f>
+        <v>0.2</v>
       </c>
       <c r="G26" s="1" t="n">
-        <f aca="false">G11/5</f>
-        <v>0.2</v>
+        <f aca="false">G11/6</f>
+        <v>1.5</v>
       </c>
       <c r="H26" s="1" t="n">
-        <f aca="false">H11/6</f>
-        <v>1.5</v>
-      </c>
-      <c r="I26" s="1" t="n">
-        <f aca="false">I11/7</f>
+        <f aca="false">H11/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="J26" s="0" t="n">
-        <f aca="false">B26+C26+D26</f>
+      <c r="I26" s="0" t="n">
+        <f aca="false">B26+C26</f>
         <v>493.5</v>
       </c>
-      <c r="K26" s="4" t="n">
-        <f aca="false">J26/L26</f>
+      <c r="J26" s="4" t="n">
+        <f aca="false">I26/K26</f>
         <v>0.905350333494948</v>
       </c>
-      <c r="L26" s="0" t="n">
-        <f aca="false">SUM(B26:I26)</f>
+      <c r="K26" s="0" t="n">
+        <f aca="false">SUM(B26:H26)</f>
         <v>545.092857142857</v>
       </c>
     </row>
@@ -2483,42 +2323,39 @@
         <v>23</v>
       </c>
       <c r="C27" s="1" t="n">
-        <v>0</v>
+        <f aca="false">C12/2</f>
+        <v>30</v>
       </c>
       <c r="D27" s="1" t="n">
-        <f aca="false">D12/2</f>
-        <v>30</v>
+        <f aca="false">D12/3</f>
+        <v>14.6666666666667</v>
       </c>
       <c r="E27" s="1" t="n">
-        <f aca="false">E12/3</f>
-        <v>14.6666666666667</v>
+        <f aca="false">E11/4</f>
+        <v>20.75</v>
       </c>
       <c r="F27" s="1" t="n">
-        <f aca="false">F11/4</f>
-        <v>20.75</v>
+        <f aca="false">F12/5</f>
+        <v>0</v>
       </c>
       <c r="G27" s="1" t="n">
-        <f aca="false">G12/5</f>
-        <v>0</v>
+        <f aca="false">G12/6</f>
+        <v>1.5</v>
       </c>
       <c r="H27" s="1" t="n">
-        <f aca="false">H12/6</f>
-        <v>1.5</v>
-      </c>
-      <c r="I27" s="1" t="n">
-        <f aca="false">I12/7</f>
+        <f aca="false">H12/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="J27" s="0" t="n">
-        <f aca="false">B27+C27+D27</f>
+      <c r="I27" s="0" t="n">
+        <f aca="false">B27+C27</f>
         <v>53</v>
       </c>
-      <c r="K27" s="4" t="n">
-        <f aca="false">J27/L27</f>
+      <c r="J27" s="4" t="n">
+        <f aca="false">I27/K27</f>
         <v>0.588499669530734</v>
       </c>
-      <c r="L27" s="0" t="n">
-        <f aca="false">SUM(B27:I27)</f>
+      <c r="K27" s="0" t="n">
+        <f aca="false">SUM(B27:H27)</f>
         <v>90.0595238095238</v>
       </c>
     </row>
@@ -2530,42 +2367,39 @@
         <v>42</v>
       </c>
       <c r="C28" s="1" t="n">
-        <v>0</v>
+        <f aca="false">C13/2</f>
+        <v>18</v>
       </c>
       <c r="D28" s="1" t="n">
-        <f aca="false">D13/2</f>
-        <v>18</v>
+        <f aca="false">D13/3</f>
+        <v>0</v>
       </c>
       <c r="E28" s="1" t="n">
-        <f aca="false">E13/3</f>
-        <v>0</v>
+        <f aca="false">E12/4</f>
+        <v>0.75</v>
       </c>
       <c r="F28" s="1" t="n">
-        <f aca="false">F12/4</f>
-        <v>0.75</v>
+        <f aca="false">F13/5</f>
+        <v>0</v>
       </c>
       <c r="G28" s="1" t="n">
-        <f aca="false">G13/5</f>
-        <v>0</v>
+        <f aca="false">G13/6</f>
+        <v>1.5</v>
       </c>
       <c r="H28" s="1" t="n">
-        <f aca="false">H13/6</f>
-        <v>1.5</v>
-      </c>
-      <c r="I28" s="1" t="n">
-        <f aca="false">I13/7</f>
+        <f aca="false">H13/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="J28" s="0" t="n">
-        <f aca="false">B28+C28+D28</f>
+      <c r="I28" s="0" t="n">
+        <f aca="false">B28+C28</f>
         <v>60</v>
       </c>
-      <c r="K28" s="4" t="n">
-        <f aca="false">J28/L28</f>
+      <c r="J28" s="4" t="n">
+        <f aca="false">I28/K28</f>
         <v>0.961648540354894</v>
       </c>
-      <c r="L28" s="0" t="n">
-        <f aca="false">SUM(B28:I28)</f>
+      <c r="K28" s="0" t="n">
+        <f aca="false">SUM(B28:H28)</f>
         <v>62.3928571428571</v>
       </c>
     </row>
@@ -2579,4 +2413,30 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
new additions to the analysis
</commit_message>
<xml_diff>
--- a/R/Dated_inscriptions_coefficient.xlsx
+++ b/R/Dated_inscriptions_coefficient.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
   <si>
     <t xml:space="preserve">Century</t>
   </si>
@@ -102,16 +102,60 @@
   </si>
   <si>
     <t xml:space="preserve">%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Století</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">méně než 0,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6. st. př. n. l.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. st. př. n. l.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. st. př. n. l.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. st. př. n. l.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. st. př. n. l.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. st. př. n. l.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. st. n. l.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. st. n. l.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. st. n. l.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. st. n. l.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. st. n. l.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="0.00%"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="168" formatCode="0%"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -142,24 +186,25 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="13"/>
-      <color rgb="FF000000"/>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
+      <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -207,7 +252,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -228,6 +273,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -242,7 +295,7 @@
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
       <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF66FF00"/>
+      <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
@@ -279,16 +332,16 @@
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3399FF"/>
+      <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FFAECF00"/>
+      <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF420E"/>
+      <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF999999"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF579D1C"/>
+      <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
@@ -300,7 +353,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -312,7 +365,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+              <a:defRPr b="1" sz="1400" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -325,7 +378,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+              <a:rPr b="1" sz="1400" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -336,7 +389,7 @@
                 </a:uFill>
                 <a:latin typeface="Arial"/>
               </a:rPr>
-              <a:t>Procentuální zastoupení šíře datace (1=datované do jednoho století, 0.125=datované do osmi století)</a:t>
+              <a:t>Procentuální zastoupení šíře intervalu datace nápisů</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -345,8 +398,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0247381640680536"/>
-          <c:y val="0.0258986696858194"/>
+          <c:x val="0.208380215131194"/>
+          <c:y val="0.0461095100864553"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -362,7 +415,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$17</c:f>
+              <c:f>Sheet1!$B$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -373,15 +426,32 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="ff420e"/>
+              <a:srgbClr val="000000"/>
             </a:solidFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:dLblPos val="ctr"/>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -391,48 +461,48 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$18:$A$28</c:f>
+              <c:f>Sheet1!$A$34:$A$44</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>6 st. př. n. l.</c:v>
+                  <c:v>6. st. př. n. l.</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5 st. př. n. l.</c:v>
+                  <c:v>5. st. př. n. l.</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4 st. př. n. l.</c:v>
+                  <c:v>4. st. př. n. l.</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3 st. př. n. l.</c:v>
+                  <c:v>3. st. př. n. l.</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2 st. př. n. l.</c:v>
+                  <c:v>2. st. př. n. l.</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1 st. př. n. l.</c:v>
+                  <c:v>1. st. př. n. l.</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1 st. n. l.</c:v>
+                  <c:v>1. st. n. l.</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2 st. n. l.</c:v>
+                  <c:v>2. st. n. l.</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3 st. n. l.</c:v>
+                  <c:v>3. st. n. l.</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4 st. n. l.</c:v>
+                  <c:v>4. st. n. l.</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5 st. n. l.</c:v>
+                  <c:v>5. st. n. l.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$18:$B$28</c:f>
+              <c:f>Sheet1!$B$34:$B$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -478,26 +548,27 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$17</c:f>
+              <c:f>Sheet1!$C$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.5</c:v>
+                  <c:v>0,5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="ff8080"/>
+              <a:srgbClr val="999999"/>
             </a:solidFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -507,48 +578,48 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$18:$A$28</c:f>
+              <c:f>Sheet1!$A$34:$A$44</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>6 st. př. n. l.</c:v>
+                  <c:v>6. st. př. n. l.</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5 st. př. n. l.</c:v>
+                  <c:v>5. st. př. n. l.</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4 st. př. n. l.</c:v>
+                  <c:v>4. st. př. n. l.</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3 st. př. n. l.</c:v>
+                  <c:v>3. st. př. n. l.</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2 st. př. n. l.</c:v>
+                  <c:v>2. st. př. n. l.</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1 st. př. n. l.</c:v>
+                  <c:v>1. st. př. n. l.</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1 st. n. l.</c:v>
+                  <c:v>1. st. n. l.</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2 st. n. l.</c:v>
+                  <c:v>2. st. n. l.</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3 st. n. l.</c:v>
+                  <c:v>3. st. n. l.</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4 st. n. l.</c:v>
+                  <c:v>4. st. n. l.</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5 st. n. l.</c:v>
+                  <c:v>5. st. n. l.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$18:$C$28</c:f>
+              <c:f>Sheet1!$C$34:$C$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -594,26 +665,27 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$17</c:f>
+              <c:f>Sheet1!$D$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.33</c:v>
+                  <c:v>méně než 0,5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="0000ff"/>
+              <a:srgbClr val="ffffff"/>
             </a:solidFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -623,48 +695,48 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$18:$A$28</c:f>
+              <c:f>Sheet1!$A$34:$A$44</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>6 st. př. n. l.</c:v>
+                  <c:v>6. st. př. n. l.</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5 st. př. n. l.</c:v>
+                  <c:v>5. st. př. n. l.</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4 st. př. n. l.</c:v>
+                  <c:v>4. st. př. n. l.</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3 st. př. n. l.</c:v>
+                  <c:v>3. st. př. n. l.</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2 st. př. n. l.</c:v>
+                  <c:v>2. st. př. n. l.</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1 st. př. n. l.</c:v>
+                  <c:v>1. st. př. n. l.</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1 st. n. l.</c:v>
+                  <c:v>1. st. n. l.</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2 st. n. l.</c:v>
+                  <c:v>2. st. n. l.</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3 st. n. l.</c:v>
+                  <c:v>3. st. n. l.</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4 st. n. l.</c:v>
+                  <c:v>4. st. n. l.</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5 st. n. l.</c:v>
+                  <c:v>5. st. n. l.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$18:$D$28</c:f>
+              <c:f>Sheet1!$D$34:$D$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -672,498 +744,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.333333333333333</c:v>
+                  <c:v>0.533333333333333</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.66666666666667</c:v>
+                  <c:v>2.11666666666667</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.66666666666667</c:v>
+                  <c:v>14.5095238095238</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.66666666666667</c:v>
+                  <c:v>15.4595238095238</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>15.5428571428571</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15.3333333333333</c:v>
+                  <c:v>47.6761904761905</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14.3333333333333</c:v>
+                  <c:v>36.4261904761905</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>29</c:v>
+                  <c:v>51.5928571428572</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14.6666666666667</c:v>
+                  <c:v>37.0595238095238</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$E$17</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.25</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="3399ff"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$18:$A$28</c:f>
-              <c:strCache>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>6 st. př. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5 st. př. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4 st. př. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3 st. př. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2 st. př. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1 st. př. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1 st. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2 st. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3 st. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4 st. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5 st. n. l.</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$E$18:$E$28</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.25</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10.5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10.25</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>30.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>20.25</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>20.75</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>20.75</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.75</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$F$17</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="aecf00"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$18:$A$28</c:f>
-              <c:strCache>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>6 st. př. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5 st. př. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4 st. př. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3 st. př. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2 st. př. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1 st. př. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1 st. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2 st. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3 st. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4 st. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5 st. n. l.</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$F$18:$F$28</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$G$17</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.16</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="66ff00"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$18:$A$28</c:f>
-              <c:strCache>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>6 st. př. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5 st. př. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4 st. př. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3 st. př. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2 st. př. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1 st. př. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1 st. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2 st. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3 st. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4 st. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5 st. n. l.</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$G$18:$G$28</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$H$17</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.125</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="579d1c"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$18:$A$28</c:f>
-              <c:strCache>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>6 st. př. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5 st. př. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4 st. př. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3 st. př. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2 st. př. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1 st. př. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1 st. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2 st. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3 st. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4 st. n. l.</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5 st. n. l.</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$H$18:$H$28</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.142857142857143</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.142857142857143</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.142857142857143</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.142857142857143</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.142857142857143</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.142857142857143</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.142857142857143</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.142857142857143</c:v>
+                  <c:v>2.39285714285714</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1171,11 +779,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="70172118"/>
-        <c:axId val="46014137"/>
+        <c:axId val="46685268"/>
+        <c:axId val="16090797"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="70172118"/>
+        <c:axId val="46685268"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1188,7 +796,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr b="1" sz="1000" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1201,7 +809,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                  <a:rPr b="1" sz="1000" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1248,14 +856,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46014137"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="16090797"/>
+        <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="46014137"/>
+        <c:axId val="16090797"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1277,7 +885,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr b="1" sz="1000" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1290,7 +898,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                  <a:rPr b="1" sz="1000" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1301,14 +909,22 @@
                     </a:uFill>
                     <a:latin typeface="Arial"/>
                   </a:rPr>
-                  <a:t>Procentuální zastoupení datovaných nápisů z daného století</a:t>
+                  <a:t>Procentuální zastoupení datovaných nápisů (celkem 2276 nápisů)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.0203429497277105"/>
+              <c:y val="0.860110470701249"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="0.00%" sourceLinked="0"/>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1323,7 +939,7 @@
           <a:bodyPr/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:defRPr b="1" sz="1000" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -1337,8 +953,8 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70172118"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="46685268"/>
+        <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -1378,16 +994,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>553320</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>143640</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19800</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>19080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>148320</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>28800</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>207720</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>162720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1395,8 +1011,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9354240" y="2256840"/>
-        <a:ext cx="7596000" cy="5087160"/>
+        <a:off x="3924720" y="4895640"/>
+        <a:ext cx="7998480" cy="5995800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1414,16 +1030,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:L28"/>
+  <dimension ref="A2:M44"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S50" activeCellId="0" sqref="S50"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S36" activeCellId="0" sqref="S36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -1962,6 +1575,8 @@
         <f aca="false">SUM(B18:H18)</f>
         <v>6</v>
       </c>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
@@ -2006,6 +1621,8 @@
         <f aca="false">SUM(B19:H19)</f>
         <v>124.033333333333</v>
       </c>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
@@ -2050,6 +1667,8 @@
         <f aca="false">SUM(B20:H20)</f>
         <v>244.616666666667</v>
       </c>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
@@ -2094,6 +1713,8 @@
         <f aca="false">SUM(B21:H21)</f>
         <v>173.509523809524</v>
       </c>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
@@ -2138,6 +1759,8 @@
         <f aca="false">SUM(B22:H22)</f>
         <v>222.459523809524</v>
       </c>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
@@ -2182,6 +1805,8 @@
         <f aca="false">SUM(B23:H23)</f>
         <v>175.042857142857</v>
       </c>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
@@ -2226,6 +1851,8 @@
         <f aca="false">SUM(B24:H24)</f>
         <v>190.67619047619</v>
       </c>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
@@ -2270,6 +1897,8 @@
         <f aca="false">SUM(B25:H25)</f>
         <v>427.42619047619</v>
       </c>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
@@ -2314,6 +1943,8 @@
         <f aca="false">SUM(B26:H26)</f>
         <v>545.092857142857</v>
       </c>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
@@ -2358,6 +1989,8 @@
         <f aca="false">SUM(B27:H27)</f>
         <v>90.0595238095238</v>
       </c>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
@@ -2402,6 +2035,262 @@
         <f aca="false">SUM(B28:H28)</f>
         <v>62.3928571428571</v>
       </c>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C34" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D34" s="6" t="n">
+        <f aca="false">D18+E18+F18+G18+H18</f>
+        <v>0</v>
+      </c>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="4"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="5" t="n">
+        <v>60</v>
+      </c>
+      <c r="C35" s="1" t="n">
+        <v>63.5</v>
+      </c>
+      <c r="D35" s="6" t="n">
+        <f aca="false">D19+E19+F19+G19+H19</f>
+        <v>0.533333333333333</v>
+      </c>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="4"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" s="5" t="n">
+        <v>168</v>
+      </c>
+      <c r="C36" s="1" t="n">
+        <v>74.5</v>
+      </c>
+      <c r="D36" s="6" t="n">
+        <f aca="false">D20+E20+F20+G20+H20</f>
+        <v>2.11666666666667</v>
+      </c>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="4"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B37" s="5" t="n">
+        <v>117</v>
+      </c>
+      <c r="C37" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="D37" s="6" t="n">
+        <f aca="false">D21+E21+F21+G21+H21</f>
+        <v>14.5095238095238</v>
+      </c>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="4"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B38" s="5" t="n">
+        <v>115</v>
+      </c>
+      <c r="C38" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="D38" s="6" t="n">
+        <f aca="false">D22+E22+F22+G22+H22</f>
+        <v>15.4595238095238</v>
+      </c>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="4"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B39" s="5" t="n">
+        <v>69</v>
+      </c>
+      <c r="C39" s="1" t="n">
+        <v>90.5</v>
+      </c>
+      <c r="D39" s="6" t="n">
+        <f aca="false">D23+E23+F23+G23+H23</f>
+        <v>15.5428571428571</v>
+      </c>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="4"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B40" s="5" t="n">
+        <v>68</v>
+      </c>
+      <c r="C40" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="D40" s="6" t="n">
+        <f aca="false">D24+E24+F24+G24+H24</f>
+        <v>47.6761904761905</v>
+      </c>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="4"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B41" s="5" t="n">
+        <v>253</v>
+      </c>
+      <c r="C41" s="1" t="n">
+        <v>138</v>
+      </c>
+      <c r="D41" s="6" t="n">
+        <f aca="false">D25+E25+F25+G25+H25</f>
+        <v>36.4261904761905</v>
+      </c>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="4"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B42" s="5" t="n">
+        <v>390</v>
+      </c>
+      <c r="C42" s="1" t="n">
+        <v>103.5</v>
+      </c>
+      <c r="D42" s="6" t="n">
+        <f aca="false">D26+E26+F26+G26+H26</f>
+        <v>51.5928571428572</v>
+      </c>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="4"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B43" s="5" t="n">
+        <v>23</v>
+      </c>
+      <c r="C43" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="D43" s="6" t="n">
+        <f aca="false">D27+E27+F27+G27+H27</f>
+        <v>37.0595238095238</v>
+      </c>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="4"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" s="5" t="n">
+        <v>42</v>
+      </c>
+      <c r="C44" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="D44" s="6" t="n">
+        <f aca="false">D28+E28+F28+G28+H28</f>
+        <v>2.39285714285714</v>
+      </c>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2422,13 +2311,13 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
test video sequence for presentation
</commit_message>
<xml_diff>
--- a/R/Dated_inscriptions_coefficient.xlsx
+++ b/R/Dated_inscriptions_coefficient.xlsx
@@ -5,11 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="CZ" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="ENG" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="64">
   <si>
     <t xml:space="preserve">Century</t>
   </si>
@@ -165,6 +165,54 @@
   </si>
   <si>
     <t xml:space="preserve">5. st. n. l.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6BC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5BC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4BC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3BC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2BC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1BC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1AD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2AD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3AD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4AD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5AD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6-8AD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5-8AD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;100 yrs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;200 yrs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;200 yrs</t>
   </si>
 </sst>
 </file>
@@ -386,7 +434,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -431,8 +479,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.140871451104101"/>
-          <c:y val="0.0271413464927741"/>
+          <c:x val="0.140868345936201"/>
+          <c:y val="0.0271432600112803"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -448,7 +496,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$32:$B$32</c:f>
+              <c:f>CZ!$B$32:$B$32</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -497,7 +545,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$33:$A$43</c:f>
+              <c:f>CZ!$A$33:$A$43</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
@@ -538,7 +586,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$33:$B$43</c:f>
+              <c:f>CZ!$B$33:$B$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -584,7 +632,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$32:$C$32</c:f>
+              <c:f>CZ!$C$32:$C$32</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -615,7 +663,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$33:$A$43</c:f>
+              <c:f>CZ!$A$33:$A$43</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
@@ -656,7 +704,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$33:$C$43</c:f>
+              <c:f>CZ!$C$33:$C$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -702,7 +750,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$32:$D$32</c:f>
+              <c:f>CZ!$D$32:$D$32</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -733,7 +781,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$33:$A$43</c:f>
+              <c:f>CZ!$A$33:$A$43</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
@@ -774,7 +822,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$33:$D$43</c:f>
+              <c:f>CZ!$D$33:$D$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -817,11 +865,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="80939135"/>
-        <c:axId val="95955231"/>
+        <c:axId val="16008651"/>
+        <c:axId val="10297480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="80939135"/>
+        <c:axId val="16008651"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -894,14 +942,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95955231"/>
+        <c:crossAx val="10297480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95955231"/>
+        <c:axId val="10297480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -956,8 +1004,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.0204061514195584"/>
-              <c:y val="0.859922453295735"/>
+              <c:x val="0.020431669087085"/>
+              <c:y val="0.859771573604061"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -991,7 +1039,603 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80939135"/>
+        <c:crossAx val="16008651"/>
+        <c:crossesAt val="1"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="1" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Percentage of dated inscriptions by centuries (n=2276)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.140918423556513"/>
+          <c:y val="0.0270937650044585"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="percentStacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>label 0</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>&lt;100 yrs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>6BC</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5BC</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4BC</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3BC</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2BC</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1BC</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1AD</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2AD</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3AD</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4AD</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5-8AD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>0</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>253</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>label 1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>&lt;200 yrs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="999999"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>6BC</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5BC</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4BC</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3BC</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2BC</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1BC</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1AD</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2AD</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3AD</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4AD</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5-8AD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>58.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>62.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>label 2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>&gt;200yrs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffffff"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>6BC</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5BC</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4BC</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3BC</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2BC</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1BC</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1AD</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2AD</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3AD</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4AD</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5-8AD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.583333333333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.783333333333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.3666666666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.2595238095238</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.7095238095238</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35.5428571428571</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>37.4261904761904</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>36.9261904761904</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>51.5928571428572</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17.0595238095238</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16.8095238095238</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:overlap val="0"/>
+        <c:axId val="89648730"/>
+        <c:axId val="56854644"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="89648730"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="1" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Století</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="DD/MM/YYYY" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="56854644"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="56854644"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="1" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="89648730"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1039,9 +1683,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>523800</xdr:colOff>
+      <xdr:colOff>523440</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>22320</xdr:rowOff>
+      <xdr:rowOff>21960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1049,8 +1693,43 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8837640" y="2046240"/>
-        <a:ext cx="7303320" cy="5106240"/>
+        <a:off x="8708040" y="2046240"/>
+        <a:ext cx="7188480" cy="5105880"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>421920</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>96120</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>523800</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>142200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="1" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="8951040" y="2046600"/>
+        <a:ext cx="7188480" cy="5248080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1070,14 +1749,14 @@
   </sheetPr>
   <dimension ref="A2:M62"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K37" activeCellId="0" sqref="K37"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.2244897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2694,14 +3373,1618 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A2:M62"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L45" activeCellId="0" sqref="L45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <sheetData/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.8061224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="2"/>
+      <c r="L2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>7.16</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <f aca="false">D3+E3+F3+G3+H3</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>124</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>170.05</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <v>187</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L4" s="1" t="n">
+        <v>190</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <f aca="false">D4+E4+F4+G4+H4</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>168</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>117</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>326.675</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <v>317</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L5" s="1" t="n">
+        <v>365</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <f aca="false">D5+E5+F5+G5+H5</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>117</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>228.225</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <v>201</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L6" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <f aca="false">D6+E6+F6+G6+H6</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>115</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>125</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>320.41</v>
+      </c>
+      <c r="J7" s="1" t="n">
+        <v>299</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" s="1" t="n">
+        <v>358</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <f aca="false">D7+E7+F7+G7+H7</f>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>122</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="H8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1" t="n">
+        <v>351.735</v>
+      </c>
+      <c r="J8" s="1" t="n">
+        <v>250</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L8" s="1" t="n">
+        <v>393</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <f aca="false">D8+E8+F8+G8+H8</f>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>94</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="H9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" s="1" t="n">
+        <v>318.62</v>
+      </c>
+      <c r="J9" s="1" t="n">
+        <v>218</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" s="1" t="n">
+        <v>356</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <f aca="false">D9+E9+F9+G9+H9</f>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>253</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>182</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="H10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" s="1" t="n">
+        <v>596.07</v>
+      </c>
+      <c r="J10" s="1" t="n">
+        <v>529</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L10" s="1" t="n">
+        <v>666</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <f aca="false">D10+E10+F10+G10+H10</f>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>390</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="H11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1" t="n">
+        <v>696.31</v>
+      </c>
+      <c r="J11" s="1" t="n">
+        <v>597</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" s="1" t="n">
+        <v>778</v>
+      </c>
+      <c r="M11" s="0" t="n">
+        <f aca="false">D11+E11+F11+G11+H11</f>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="H12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" s="1" t="n">
+        <v>125.3</v>
+      </c>
+      <c r="J12" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L12" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="M12" s="0" t="n">
+        <f aca="false">D12+E12+F12+G12+H12</f>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="H13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" s="1" t="n">
+        <v>118.14</v>
+      </c>
+      <c r="J13" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L13" s="1" t="n">
+        <v>132</v>
+      </c>
+      <c r="M13" s="0" t="n">
+        <f aca="false">D13+E13+F13+G13+H13</f>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="n">
+        <f aca="false">SUM(B3:B14)</f>
+        <v>1320</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <f aca="false">SUM(C3:C14)</f>
+        <v>837</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="E17" s="1" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="G17" s="1" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="H17" s="1" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="K17" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <f aca="false">C3/2</f>
+        <v>1.5</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <f aca="false">D3/3</f>
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E18" s="1" t="n">
+        <f aca="false">E3/4</f>
+        <v>0.25</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <f aca="false">B18+C18</f>
+        <v>4.5</v>
+      </c>
+      <c r="J18" s="5" t="n">
+        <f aca="false">I18/K18</f>
+        <v>0.885245901639344</v>
+      </c>
+      <c r="K18" s="0" t="n">
+        <f aca="false">SUM(B18:H18)</f>
+        <v>5.08333333333333</v>
+      </c>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <f aca="false">C4/2</f>
+        <v>62</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <f aca="false">D4/3</f>
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E19" s="1" t="n">
+        <f aca="false">E4/4</f>
+        <v>0.25</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <f aca="false">F4/5</f>
+        <v>0.2</v>
+      </c>
+      <c r="G19" s="1" t="n">
+        <f aca="false">G4/6</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="1" t="n">
+        <f aca="false">H4/7</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <f aca="false">B19+C19</f>
+        <v>122</v>
+      </c>
+      <c r="J19" s="5" t="n">
+        <f aca="false">I19/K19</f>
+        <v>0.993620198181078</v>
+      </c>
+      <c r="K19" s="0" t="n">
+        <f aca="false">SUM(B19:H19)</f>
+        <v>122.783333333333</v>
+      </c>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="1" t="n">
+        <v>168</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <f aca="false">C5/2</f>
+        <v>58.5</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <f aca="false">D5/3</f>
+        <v>1.66666666666667</v>
+      </c>
+      <c r="E20" s="1" t="n">
+        <f aca="false">E5/4</f>
+        <v>10.5</v>
+      </c>
+      <c r="F20" s="1" t="n">
+        <f aca="false">F5/5</f>
+        <v>0.2</v>
+      </c>
+      <c r="G20" s="1" t="n">
+        <f aca="false">G5/6</f>
+        <v>0</v>
+      </c>
+      <c r="H20" s="1" t="n">
+        <f aca="false">H5/7</f>
+        <v>0</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <f aca="false">B20+C20</f>
+        <v>226.5</v>
+      </c>
+      <c r="J20" s="5" t="n">
+        <f aca="false">I20/K20</f>
+        <v>0.948227742115546</v>
+      </c>
+      <c r="K20" s="0" t="n">
+        <f aca="false">SUM(B20:H20)</f>
+        <v>238.866666666667</v>
+      </c>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="1" t="n">
+        <v>117</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <f aca="false">C6/2</f>
+        <v>29.5</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <f aca="false">D6/3</f>
+        <v>3.66666666666667</v>
+      </c>
+      <c r="E21" s="1" t="n">
+        <f aca="false">E6/4</f>
+        <v>10.25</v>
+      </c>
+      <c r="F21" s="1" t="n">
+        <f aca="false">F6/5</f>
+        <v>0.2</v>
+      </c>
+      <c r="G21" s="1" t="n">
+        <f aca="false">G6/6</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="1" t="n">
+        <f aca="false">H6/7</f>
+        <v>0.142857142857143</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <f aca="false">B21+C21</f>
+        <v>146.5</v>
+      </c>
+      <c r="J21" s="5" t="n">
+        <f aca="false">I21/K21</f>
+        <v>0.911299041751211</v>
+      </c>
+      <c r="K21" s="0" t="n">
+        <f aca="false">SUM(B21:H21)</f>
+        <v>160.759523809524</v>
+      </c>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="1" t="n">
+        <v>115</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <f aca="false">C7/2</f>
+        <v>62.5</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <f aca="false">D7/3</f>
+        <v>4.66666666666667</v>
+      </c>
+      <c r="E22" s="1" t="n">
+        <f aca="false">E7/4</f>
+        <v>10.5</v>
+      </c>
+      <c r="F22" s="1" t="n">
+        <f aca="false">F7/5</f>
+        <v>0.4</v>
+      </c>
+      <c r="G22" s="1" t="n">
+        <f aca="false">G7/6</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="1" t="n">
+        <f aca="false">H7/7</f>
+        <v>0.142857142857143</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <f aca="false">B22+C22</f>
+        <v>177.5</v>
+      </c>
+      <c r="J22" s="5" t="n">
+        <f aca="false">I22/K22</f>
+        <v>0.918691773056637</v>
+      </c>
+      <c r="K22" s="0" t="n">
+        <f aca="false">SUM(B22:H22)</f>
+        <v>193.209523809524</v>
+      </c>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <f aca="false">C8/2</f>
+        <v>28</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <f aca="false">D8/3</f>
+        <v>3</v>
+      </c>
+      <c r="E23" s="1" t="n">
+        <f aca="false">E8/4</f>
+        <v>30.5</v>
+      </c>
+      <c r="F23" s="1" t="n">
+        <f aca="false">F8/5</f>
+        <v>0.4</v>
+      </c>
+      <c r="G23" s="1" t="n">
+        <f aca="false">G8/6</f>
+        <v>1.5</v>
+      </c>
+      <c r="H23" s="1" t="n">
+        <f aca="false">H8/7</f>
+        <v>0.142857142857143</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <f aca="false">B23+C23</f>
+        <v>97</v>
+      </c>
+      <c r="J23" s="5" t="n">
+        <f aca="false">I23/K23</f>
+        <v>0.731838758353093</v>
+      </c>
+      <c r="K23" s="0" t="n">
+        <f aca="false">SUM(B23:H23)</f>
+        <v>132.542857142857</v>
+      </c>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <f aca="false">C9/2</f>
+        <v>47</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <f aca="false">D9/3</f>
+        <v>15.3333333333333</v>
+      </c>
+      <c r="E24" s="1" t="n">
+        <f aca="false">E9/4</f>
+        <v>20.25</v>
+      </c>
+      <c r="F24" s="1" t="n">
+        <f aca="false">F9/5</f>
+        <v>0.2</v>
+      </c>
+      <c r="G24" s="1" t="n">
+        <f aca="false">G9/6</f>
+        <v>1.5</v>
+      </c>
+      <c r="H24" s="1" t="n">
+        <f aca="false">H9/7</f>
+        <v>0.142857142857143</v>
+      </c>
+      <c r="I24" s="0" t="n">
+        <f aca="false">B24+C24</f>
+        <v>115</v>
+      </c>
+      <c r="J24" s="5" t="n">
+        <f aca="false">I24/K24</f>
+        <v>0.754463518642903</v>
+      </c>
+      <c r="K24" s="0" t="n">
+        <f aca="false">SUM(B24:H24)</f>
+        <v>152.42619047619</v>
+      </c>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="1" t="n">
+        <v>253</v>
+      </c>
+      <c r="C25" s="1" t="n">
+        <f aca="false">C10/2</f>
+        <v>91</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <f aca="false">D10/3</f>
+        <v>14.3333333333333</v>
+      </c>
+      <c r="E25" s="1" t="n">
+        <f aca="false">E10/4</f>
+        <v>20.75</v>
+      </c>
+      <c r="F25" s="1" t="n">
+        <f aca="false">F10/5</f>
+        <v>0.2</v>
+      </c>
+      <c r="G25" s="1" t="n">
+        <f aca="false">G10/6</f>
+        <v>1.5</v>
+      </c>
+      <c r="H25" s="1" t="n">
+        <f aca="false">H10/7</f>
+        <v>0.142857142857143</v>
+      </c>
+      <c r="I25" s="0" t="n">
+        <f aca="false">B25+C25</f>
+        <v>344</v>
+      </c>
+      <c r="J25" s="5" t="n">
+        <f aca="false">I25/K25</f>
+        <v>0.903062085518379</v>
+      </c>
+      <c r="K25" s="0" t="n">
+        <f aca="false">SUM(B25:H25)</f>
+        <v>380.92619047619</v>
+      </c>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="1" t="n">
+        <v>390</v>
+      </c>
+      <c r="C26" s="1" t="n">
+        <f aca="false">C11/2</f>
+        <v>12</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <f aca="false">D11/3</f>
+        <v>29</v>
+      </c>
+      <c r="E26" s="1" t="n">
+        <f aca="false">E11/4</f>
+        <v>20.75</v>
+      </c>
+      <c r="F26" s="1" t="n">
+        <f aca="false">F11/5</f>
+        <v>0.2</v>
+      </c>
+      <c r="G26" s="1" t="n">
+        <f aca="false">G11/6</f>
+        <v>1.5</v>
+      </c>
+      <c r="H26" s="1" t="n">
+        <f aca="false">H11/7</f>
+        <v>0.142857142857143</v>
+      </c>
+      <c r="I26" s="0" t="n">
+        <f aca="false">B26+C26</f>
+        <v>402</v>
+      </c>
+      <c r="J26" s="5" t="n">
+        <f aca="false">I26/K26</f>
+        <v>0.886257342172811</v>
+      </c>
+      <c r="K26" s="0" t="n">
+        <f aca="false">SUM(B26:H26)</f>
+        <v>453.592857142857</v>
+      </c>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="C27" s="1" t="n">
+        <f aca="false">C12/2</f>
+        <v>17.5</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <f aca="false">D12/3</f>
+        <v>14.6666666666667</v>
+      </c>
+      <c r="E27" s="1" t="n">
+        <f aca="false">E12/4</f>
+        <v>0.75</v>
+      </c>
+      <c r="F27" s="1" t="n">
+        <f aca="false">F12/5</f>
+        <v>0</v>
+      </c>
+      <c r="G27" s="1" t="n">
+        <f aca="false">G12/6</f>
+        <v>1.5</v>
+      </c>
+      <c r="H27" s="1" t="n">
+        <f aca="false">H12/7</f>
+        <v>0.142857142857143</v>
+      </c>
+      <c r="I27" s="0" t="n">
+        <f aca="false">B27+C27</f>
+        <v>40.5</v>
+      </c>
+      <c r="J27" s="5" t="n">
+        <f aca="false">I27/K27</f>
+        <v>0.703619441571872</v>
+      </c>
+      <c r="K27" s="0" t="n">
+        <f aca="false">SUM(B27:H27)</f>
+        <v>57.5595238095238</v>
+      </c>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="C28" s="1" t="n">
+        <f aca="false">C13/2</f>
+        <v>8</v>
+      </c>
+      <c r="D28" s="1" t="n">
+        <f aca="false">D13/3</f>
+        <v>14.6666666666667</v>
+      </c>
+      <c r="E28" s="1" t="n">
+        <f aca="false">E13/4</f>
+        <v>0.5</v>
+      </c>
+      <c r="F28" s="1" t="n">
+        <f aca="false">F13/5</f>
+        <v>0</v>
+      </c>
+      <c r="G28" s="1" t="n">
+        <f aca="false">G13/6</f>
+        <v>1.5</v>
+      </c>
+      <c r="H28" s="1" t="n">
+        <f aca="false">H13/7</f>
+        <v>0.142857142857143</v>
+      </c>
+      <c r="I28" s="0" t="n">
+        <f aca="false">B28+C28</f>
+        <v>50</v>
+      </c>
+      <c r="J28" s="5" t="n">
+        <f aca="false">I28/K28</f>
+        <v>0.74839629365645</v>
+      </c>
+      <c r="K28" s="0" t="n">
+        <f aca="false">SUM(B28:H28)</f>
+        <v>66.8095238095238</v>
+      </c>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="0" t="n">
+        <f aca="false">SUM(B18:B28)</f>
+        <v>1308</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <f aca="false">SUM(C18:C28)</f>
+        <v>417.5</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <f aca="false">SUM(D18:D28)</f>
+        <v>101.666666666667</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <f aca="false">SUM(E18:E28)</f>
+        <v>125.25</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <f aca="false">SUM(F18:F28)</f>
+        <v>2</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <f aca="false">SUM(G18:G28)</f>
+        <v>9</v>
+      </c>
+      <c r="H29" s="0" t="n">
+        <f aca="false">SUM(H18:H28)</f>
+        <v>1.14285714285714</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C33" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D33" s="6" t="n">
+        <f aca="false">D18+E18+F18+G18+H18</f>
+        <v>0.583333333333333</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <f aca="false">B33+C33+D33</f>
+        <v>6.58333333333333</v>
+      </c>
+      <c r="F33" s="7" t="n">
+        <f aca="false">(B33+C33)/E33</f>
+        <v>0.911392405063291</v>
+      </c>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="5"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" s="4" t="n">
+        <v>60</v>
+      </c>
+      <c r="C34" s="1" t="n">
+        <f aca="false">C19</f>
+        <v>62</v>
+      </c>
+      <c r="D34" s="6" t="n">
+        <f aca="false">D19+E19+F19+G19+H19</f>
+        <v>0.783333333333333</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <f aca="false">B34+C34+D34</f>
+        <v>122.783333333333</v>
+      </c>
+      <c r="F34" s="7" t="n">
+        <f aca="false">(B34+C34)/E34</f>
+        <v>0.993620198181078</v>
+      </c>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="5"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" s="4" t="n">
+        <v>168</v>
+      </c>
+      <c r="C35" s="1" t="n">
+        <f aca="false">C20</f>
+        <v>58.5</v>
+      </c>
+      <c r="D35" s="6" t="n">
+        <f aca="false">D20+E20+F20+G20+H20</f>
+        <v>12.3666666666667</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <f aca="false">B35+C35+D35</f>
+        <v>238.866666666667</v>
+      </c>
+      <c r="F35" s="7" t="n">
+        <f aca="false">(B35+C35)/E35</f>
+        <v>0.948227742115546</v>
+      </c>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="5"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" s="4" t="n">
+        <v>117</v>
+      </c>
+      <c r="C36" s="1" t="n">
+        <f aca="false">C21</f>
+        <v>29.5</v>
+      </c>
+      <c r="D36" s="6" t="n">
+        <f aca="false">D21+E21+F21+G21+H21</f>
+        <v>14.2595238095238</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <f aca="false">B36+C36+D36</f>
+        <v>160.759523809524</v>
+      </c>
+      <c r="F36" s="7" t="n">
+        <f aca="false">(B36+C36)/E36</f>
+        <v>0.911299041751211</v>
+      </c>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="5"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" s="4" t="n">
+        <v>115</v>
+      </c>
+      <c r="C37" s="1" t="n">
+        <f aca="false">C22</f>
+        <v>62.5</v>
+      </c>
+      <c r="D37" s="6" t="n">
+        <f aca="false">D22+E22+F22+G22+H22</f>
+        <v>15.7095238095238</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <f aca="false">B37+C37+D37</f>
+        <v>193.209523809524</v>
+      </c>
+      <c r="F37" s="7" t="n">
+        <f aca="false">(B37+C37)/E37</f>
+        <v>0.918691773056637</v>
+      </c>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="5"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38" s="4" t="n">
+        <v>69</v>
+      </c>
+      <c r="C38" s="1" t="n">
+        <f aca="false">C23</f>
+        <v>28</v>
+      </c>
+      <c r="D38" s="6" t="n">
+        <f aca="false">D23+E23+F23+G23+H23</f>
+        <v>35.5428571428571</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <f aca="false">B38+C38+D38</f>
+        <v>132.542857142857</v>
+      </c>
+      <c r="F38" s="7" t="n">
+        <f aca="false">(B38+C38)/E38</f>
+        <v>0.731838758353093</v>
+      </c>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="5"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39" s="4" t="n">
+        <v>68</v>
+      </c>
+      <c r="C39" s="1" t="n">
+        <f aca="false">C24</f>
+        <v>47</v>
+      </c>
+      <c r="D39" s="6" t="n">
+        <f aca="false">D24+E24+F24+G24+H24</f>
+        <v>37.4261904761905</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <f aca="false">B39+C39+D39</f>
+        <v>152.42619047619</v>
+      </c>
+      <c r="F39" s="7" t="n">
+        <f aca="false">(B39+C39)/E39</f>
+        <v>0.754463518642903</v>
+      </c>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="5"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40" s="4" t="n">
+        <v>253</v>
+      </c>
+      <c r="C40" s="1" t="n">
+        <f aca="false">C25</f>
+        <v>91</v>
+      </c>
+      <c r="D40" s="6" t="n">
+        <f aca="false">D25+E25+F25+G25+H25</f>
+        <v>36.9261904761905</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <f aca="false">B40+C40+D40</f>
+        <v>380.92619047619</v>
+      </c>
+      <c r="F40" s="7" t="n">
+        <f aca="false">(B40+C40)/E40</f>
+        <v>0.903062085518379</v>
+      </c>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="5"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B41" s="4" t="n">
+        <v>390</v>
+      </c>
+      <c r="C41" s="1" t="n">
+        <f aca="false">C26</f>
+        <v>12</v>
+      </c>
+      <c r="D41" s="6" t="n">
+        <f aca="false">D26+E26+F26+G26+H26</f>
+        <v>51.5928571428572</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <f aca="false">B41+C41+D41</f>
+        <v>453.592857142857</v>
+      </c>
+      <c r="F41" s="7" t="n">
+        <f aca="false">(B41+C41)/E41</f>
+        <v>0.886257342172811</v>
+      </c>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="5"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B42" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="C42" s="1" t="n">
+        <f aca="false">C27</f>
+        <v>17.5</v>
+      </c>
+      <c r="D42" s="6" t="n">
+        <f aca="false">D27+E27+F27+G27+H27</f>
+        <v>17.0595238095238</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <f aca="false">B42+C42+D42</f>
+        <v>57.5595238095238</v>
+      </c>
+      <c r="F42" s="7" t="n">
+        <f aca="false">(B42+C42)/E42</f>
+        <v>0.703619441571872</v>
+      </c>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="5"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B43" s="4" t="n">
+        <v>42</v>
+      </c>
+      <c r="C43" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="D43" s="6" t="n">
+        <f aca="false">D28+E28+F28+G28+H28</f>
+        <v>16.8095238095238</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <f aca="false">B43+C43+D43</f>
+        <v>67.8095238095238</v>
+      </c>
+      <c r="F43" s="7" t="n">
+        <f aca="false">(B43+C43)/E43</f>
+        <v>0.752106741573034</v>
+      </c>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="5"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="4"/>
+      <c r="B44" s="0" t="n">
+        <f aca="false">SUM(B33:B43)</f>
+        <v>1308</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <f aca="false">SUM(C33:C43)</f>
+        <v>420</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <f aca="false">SUM(D33:D43)</f>
+        <v>239.059523809524</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <f aca="false">SUM(B44:D44)</f>
+        <v>1967.05952380952</v>
+      </c>
+      <c r="F44" s="7" t="n">
+        <f aca="false">AVERAGE(F33:F43)</f>
+        <v>0.855870822545441</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B51" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C51" s="1" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B52" s="4" t="n">
+        <v>60</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B53" s="4" t="n">
+        <v>168</v>
+      </c>
+      <c r="C53" s="0" t="n">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B54" s="4" t="n">
+        <v>117</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B55" s="4" t="n">
+        <v>115</v>
+      </c>
+      <c r="C55" s="0" t="n">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B56" s="4" t="n">
+        <v>69</v>
+      </c>
+      <c r="C56" s="0" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B57" s="4" t="n">
+        <v>68</v>
+      </c>
+      <c r="C57" s="0" t="n">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B58" s="4" t="n">
+        <v>253</v>
+      </c>
+      <c r="C58" s="0" t="n">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B59" s="4" t="n">
+        <v>390</v>
+      </c>
+      <c r="C59" s="0" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B60" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="C60" s="0" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B61" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="C61" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B62" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C62" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2709,5 +4992,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>